<commit_message>
add tree and accuracy
</commit_message>
<xml_diff>
--- a/Data vessel.xlsx
+++ b/Data vessel.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\KULIAH\SEMESTER-4\KECERDASAN BUATAN\Tubes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A7A2AB0-F74D-4F5D-8207-6E730DBE826C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3641C580-CAAF-4344-9BE9-DF287F969247}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{09640E99-5C45-4F74-8C2F-D151B28F5FA2}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{09640E99-5C45-4F74-8C2F-D151B28F5FA2}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Data Kapal" sheetId="1" r:id="rId1"/>
+    <sheet name="Pediksi Akurasi" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="89">
   <si>
     <t>NORDIKA DESGAGNES</t>
   </si>
@@ -261,6 +262,48 @@
   </si>
   <si>
     <t>EUROPA</t>
+  </si>
+  <si>
+    <t>DHT SUNDARBANS</t>
+  </si>
+  <si>
+    <t>SEAWAYS CAPE HENRY</t>
+  </si>
+  <si>
+    <t>DELTA AMAZON</t>
+  </si>
+  <si>
+    <t>TANTO SALAM</t>
+  </si>
+  <si>
+    <t>PO LIBERTE</t>
+  </si>
+  <si>
+    <t>NORTHERN RANGER</t>
+  </si>
+  <si>
+    <t>Passenger/General Cargo Ship</t>
+  </si>
+  <si>
+    <t>TORM LAURA</t>
+  </si>
+  <si>
+    <t>Chemical/Oil Products</t>
+  </si>
+  <si>
+    <t>SEABOURN SOJOURN</t>
+  </si>
+  <si>
+    <t>NORCON GALATEA</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Passenger/General Cargo Ship</t>
+  </si>
+  <si>
+    <t>CHI-CHEEMAUN</t>
+  </si>
+  <si>
+    <t>Passenger/Ro-Ro Cargo</t>
   </si>
 </sst>
 </file>
@@ -302,7 +345,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -315,6 +358,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -652,8 +698,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF3E39C3-9534-479A-93E5-5FC014DB1DF0}">
   <dimension ref="A1:J163"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2459,4 +2505,379 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D04D01A4-28AE-4D01-A230-8A13650E766A}">
+  <dimension ref="A1:J11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="8.88671875" customWidth="1"/>
+    <col min="2" max="2" width="25.44140625" customWidth="1"/>
+    <col min="3" max="3" width="25.77734375" customWidth="1"/>
+    <col min="4" max="9" width="19.21875" customWidth="1"/>
+    <col min="10" max="10" width="14.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D2">
+        <v>2019</v>
+      </c>
+      <c r="E2">
+        <v>5</v>
+      </c>
+      <c r="F2">
+        <v>10461</v>
+      </c>
+      <c r="G2">
+        <v>11164</v>
+      </c>
+      <c r="H2">
+        <v>137</v>
+      </c>
+      <c r="I2">
+        <v>23</v>
+      </c>
+      <c r="J2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3">
+        <v>2012</v>
+      </c>
+      <c r="E3">
+        <v>12</v>
+      </c>
+      <c r="F3">
+        <v>161513</v>
+      </c>
+      <c r="G3">
+        <v>318123</v>
+      </c>
+      <c r="H3">
+        <v>333</v>
+      </c>
+      <c r="I3">
+        <v>60</v>
+      </c>
+      <c r="J3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4">
+        <v>2016</v>
+      </c>
+      <c r="E4">
+        <v>8</v>
+      </c>
+      <c r="F4">
+        <v>161319</v>
+      </c>
+      <c r="G4">
+        <v>300932</v>
+      </c>
+      <c r="H4">
+        <v>333</v>
+      </c>
+      <c r="I4">
+        <v>60</v>
+      </c>
+      <c r="J4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>80</v>
+      </c>
+      <c r="C5" t="s">
+        <v>81</v>
+      </c>
+      <c r="D5">
+        <v>1986</v>
+      </c>
+      <c r="E5">
+        <v>38</v>
+      </c>
+      <c r="F5">
+        <v>2573</v>
+      </c>
+      <c r="G5">
+        <v>662</v>
+      </c>
+      <c r="H5">
+        <v>72</v>
+      </c>
+      <c r="I5">
+        <v>16</v>
+      </c>
+      <c r="J5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>85</v>
+      </c>
+      <c r="C6" t="s">
+        <v>86</v>
+      </c>
+      <c r="D6">
+        <v>1968</v>
+      </c>
+      <c r="E6">
+        <v>56</v>
+      </c>
+      <c r="F6">
+        <v>387</v>
+      </c>
+      <c r="G6">
+        <v>179</v>
+      </c>
+      <c r="H6">
+        <v>41</v>
+      </c>
+      <c r="I6">
+        <v>11</v>
+      </c>
+      <c r="J6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7">
+        <v>2023</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>47653</v>
+      </c>
+      <c r="G7">
+        <v>8850</v>
+      </c>
+      <c r="H7">
+        <v>230</v>
+      </c>
+      <c r="I7">
+        <v>31</v>
+      </c>
+      <c r="J7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>84</v>
+      </c>
+      <c r="C8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8">
+        <v>2010</v>
+      </c>
+      <c r="E8">
+        <v>14</v>
+      </c>
+      <c r="F8">
+        <v>32477</v>
+      </c>
+      <c r="G8">
+        <v>3780</v>
+      </c>
+      <c r="H8">
+        <v>198</v>
+      </c>
+      <c r="I8">
+        <v>26</v>
+      </c>
+      <c r="J8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>77</v>
+      </c>
+      <c r="C9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9">
+        <v>2015</v>
+      </c>
+      <c r="E9">
+        <v>9</v>
+      </c>
+      <c r="F9">
+        <v>166178</v>
+      </c>
+      <c r="G9">
+        <v>319896</v>
+      </c>
+      <c r="H9">
+        <v>333</v>
+      </c>
+      <c r="I9">
+        <v>60</v>
+      </c>
+      <c r="J9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>87</v>
+      </c>
+      <c r="C10" t="s">
+        <v>88</v>
+      </c>
+      <c r="D10">
+        <v>1974</v>
+      </c>
+      <c r="E10">
+        <v>50</v>
+      </c>
+      <c r="F10">
+        <v>6991</v>
+      </c>
+      <c r="G10">
+        <v>855</v>
+      </c>
+      <c r="H10">
+        <v>111</v>
+      </c>
+      <c r="I10">
+        <v>19</v>
+      </c>
+      <c r="J10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>82</v>
+      </c>
+      <c r="C11" t="s">
+        <v>83</v>
+      </c>
+      <c r="D11">
+        <v>2008</v>
+      </c>
+      <c r="E11">
+        <v>16</v>
+      </c>
+      <c r="F11">
+        <v>29300</v>
+      </c>
+      <c r="G11">
+        <v>53160</v>
+      </c>
+      <c r="H11">
+        <v>183</v>
+      </c>
+      <c r="I11">
+        <v>32</v>
+      </c>
+      <c r="J11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>